<commit_message>
Changing the input val for action inputs to 2 with new const ACTION_INPUT and moving val of OUTPUT to 3 to distinguish different input locations in the database
</commit_message>
<xml_diff>
--- a/docs/database_modell/Datenbank-Tabellen.xlsx
+++ b/docs/database_modell/Datenbank-Tabellen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Projekt\Automation_test_env\docs\database_modell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C545C7-67AB-4E2B-BC7B-4E91ACA276DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D8D354-C184-45D8-A41E-B8411CACF5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenbank Tabellen" sheetId="1" r:id="rId1"/>
@@ -657,10 +657,6 @@
     <t>wird aus der YAML-Datei bei Eingangsparametern erstellt wenn es Verknüpfungen von Entitäten gibt</t>
   </si>
   <si>
-    <t>Rolle der Entity innerhalb der Automation: 
-0  Start-, 1 Eingangs- und 2  Ausgangsparameter</t>
-  </si>
-  <si>
     <r>
       <t>a_id</t>
     </r>
@@ -711,12 +707,17 @@
     <t xml:space="preserve">Eigenschaft, die die Art der Ausführung beschreibt
 0 einzeln, 1 simultan, 2 wiederholt </t>
   </si>
+  <si>
+    <t>Rolle der Entity innerhalb der Automation: 
+0  Start-, 1 Eingangs-,  2  Aktion-Eingangs- und 
+3  Ausgangsparameter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,13 +840,6 @@
       <color rgb="FFFB872E"/>
       <name val="Cascadia Code"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1004,7 +998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1081,10 +1075,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1099,23 +1096,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1468,8 +1456,8 @@
   </sheetPr>
   <dimension ref="B2:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,36 +1484,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="F2" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="J2" s="28" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="J2" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="N2" s="28" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="N2" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="R2" s="28" t="s">
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="R2" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="V2" s="28" t="s">
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="V2" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
@@ -1537,13 +1525,13 @@
       <c r="D3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="26" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="10" t="s">
@@ -1594,9 +1582,9 @@
         <v>105</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>126</v>
       </c>
       <c r="H4" s="11" t="s">
@@ -1650,9 +1638,9 @@
         <v>43</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G5" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H5" s="11" t="s">
@@ -1708,10 +1696,10 @@
       <c r="F6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="35" t="s">
+      <c r="G6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>103</v>
       </c>
       <c r="J6" s="19" t="s">
@@ -1746,10 +1734,10 @@
       <c r="F7" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="7" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1763,13 +1751,13 @@
       <c r="D8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="7" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1783,13 +1771,13 @@
       <c r="D9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="7" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1808,31 +1796,31 @@
       <c r="B12" s="18"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="F13" s="30" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="F13" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="J13" s="30" t="s">
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="J13" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="N13" s="30" t="s">
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="N13" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="R13" s="30" t="s">
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="R13" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
@@ -2085,19 +2073,19 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="F24" s="26" t="s">
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="F24" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
@@ -2167,7 +2155,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>22</v>
@@ -2280,6 +2268,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="V2:X2"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="F13:H13"/>
@@ -2289,11 +2282,6 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="N2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2317,11 +2305,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2437,11 +2425,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2513,11 +2501,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2578,11 +2566,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2622,7 +2610,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
@@ -2673,13 +2661,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2710,11 +2698,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2833,11 +2821,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -2921,7 +2909,7 @@
         <v>82</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>80</v>
@@ -2955,11 +2943,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
@@ -3091,8 +3079,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,11 +3091,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -3142,12 +3130,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>148</v>
+      <c r="B5" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>103</v>
@@ -3212,11 +3200,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -3288,11 +3276,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -3353,11 +3341,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -3418,11 +3406,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -3494,11 +3482,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">

</xml_diff>